<commit_message>
Actualización de estilos para focalizadores y márgenes derechos
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/Desarrollo de software/Python/Guia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/Proyectos/Guía impresa/Posgrados (plantilla amarilla)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C30625F-057D-9E45-AF04-B2C717BD80A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C34F70-1962-3F43-9C94-8CBA552BDEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4880" yWindow="760" windowWidth="25480" windowHeight="18660" xr2:uid="{81AB655D-E2F9-5747-8328-0D5F0F7CE3C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Código Banner</t>
   </si>
@@ -135,12 +135,6 @@
     <t>Loja</t>
   </si>
   <si>
-    <t>Ciencias Sociales, Educación y Humanidades</t>
-  </si>
-  <si>
-    <t>Maestría profesional</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -150,34 +144,43 @@
     <t>Total 144: ACD_32 APE_16 AA_96</t>
   </si>
   <si>
-    <t>EDUC_7094</t>
-  </si>
-  <si>
-    <t>Una Nueva Mirada a la Orientación y Asesoramiento Familiar</t>
-  </si>
-  <si>
-    <t>Beltrán Guevara Patricia Maricela</t>
-  </si>
-  <si>
-    <t>pmbeltran@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Maestría en educación con mención en Orientación Familiar</t>
-  </si>
-  <si>
-    <t>Carrera Herrera Xiomara Paola</t>
-  </si>
-  <si>
-    <t>xpcarrera@utpl.edu.ec</t>
-  </si>
-  <si>
     <t>Unidad de Formación Disciplinar Avanzada</t>
   </si>
   <si>
-    <t>https://utpl.instructure.com/courses/56814</t>
-  </si>
-  <si>
-    <t>EDUC_7094_NLG_META</t>
+    <t>SIST_7014</t>
+  </si>
+  <si>
+    <t>Bases de Datos Geoespaciales</t>
+  </si>
+  <si>
+    <t>Pucha Cofrep Franz Leonardo</t>
+  </si>
+  <si>
+    <t>fapucha@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Ingenierías y Arquitectura</t>
+  </si>
+  <si>
+    <t>Especialización en Gestión de Geoinformación con mención en Proyectos de Ingeniería</t>
+  </si>
+  <si>
+    <t>González Jaramillo Víctor Hugo</t>
+  </si>
+  <si>
+    <t>vhgonzalez@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Especialización</t>
+  </si>
+  <si>
+    <t>https://utpl.instructure.com/courses/72916</t>
+  </si>
+  <si>
+    <t>SIST_7014_META</t>
+  </si>
+  <si>
+    <t>180625 Código banner incorrecto</t>
   </si>
 </sst>
 </file>
@@ -581,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203FE6DB-C04A-E24B-B012-CF294DC0B84C}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AC2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29:R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +681,7 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -687,28 +690,28 @@
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="I2" s="2">
-        <v>1103442891</v>
+        <v>1104483498</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>41</v>
@@ -716,29 +719,29 @@
       <c r="M2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="5" t="s">
         <v>43</v>
       </c>
       <c r="O2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P2" s="2">
         <v>2</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2">
+        <v>2</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="U2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>45</v>
@@ -747,21 +750,24 @@
       <c r="X2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="2"/>
+      <c r="Y2" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AB2" s="3">
-        <v>45855</v>
+        <v>45841</v>
       </c>
       <c r="AC2" s="3">
-        <v>45855</v>
+        <v>45841</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" xr:uid="{41098D46-CA91-B346-9418-67A8C8CF092A}"/>
+    <hyperlink ref="N2" r:id="rId1" display="mailto:vhgonzalez@utpl.edu.ec" xr:uid="{B2A1C3AF-0E8D-1649-8C1A-3C5136D6647F}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{5C99694D-E6EE-5541-9058-BC50378FB35F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Utilización de clases break-before y break-after actualizadas (sin page) y ajuste de tablas
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/Proyectos/Guía impresa/Posgrados (plantilla amarilla)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/GitHub/GD-Posgrados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C34F70-1962-3F43-9C94-8CBA552BDEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAF9D05-312A-4645-9E50-7E0F29FCE398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4880" yWindow="760" windowWidth="25480" windowHeight="18660" xr2:uid="{81AB655D-E2F9-5747-8328-0D5F0F7CE3C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Código Banner</t>
   </si>
@@ -141,46 +141,43 @@
     <t>Formativo</t>
   </si>
   <si>
+    <t>Unidad de Formación Disciplinar Avanzada</t>
+  </si>
+  <si>
+    <t>EDUC_7094</t>
+  </si>
+  <si>
+    <t>Una Nueva Mirada a la Orientación y Asesoramiento Familiar</t>
+  </si>
+  <si>
+    <t>Beltrán Guevara Patricia Maricela</t>
+  </si>
+  <si>
+    <t>pmbeltran@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Ciencias Sociales, Educación y Humanidades</t>
+  </si>
+  <si>
+    <t>Maestría en Educación con Mención en Orientación Familiar</t>
+  </si>
+  <si>
+    <t>Carrera Herrera Xiomara Paola</t>
+  </si>
+  <si>
+    <t>xpcarrera@utpl.edu.ec</t>
+  </si>
+  <si>
     <t>Total 144: ACD_32 APE_16 AA_96</t>
   </si>
   <si>
-    <t>Unidad de Formación Disciplinar Avanzada</t>
-  </si>
-  <si>
-    <t>SIST_7014</t>
-  </si>
-  <si>
-    <t>Bases de Datos Geoespaciales</t>
-  </si>
-  <si>
-    <t>Pucha Cofrep Franz Leonardo</t>
-  </si>
-  <si>
-    <t>fapucha@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Ingenierías y Arquitectura</t>
-  </si>
-  <si>
-    <t>Especialización en Gestión de Geoinformación con mención en Proyectos de Ingeniería</t>
-  </si>
-  <si>
-    <t>González Jaramillo Víctor Hugo</t>
-  </si>
-  <si>
-    <t>vhgonzalez@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Especialización</t>
-  </si>
-  <si>
-    <t>https://utpl.instructure.com/courses/72916</t>
-  </si>
-  <si>
-    <t>SIST_7014_META</t>
-  </si>
-  <si>
-    <t>180625 Código banner incorrecto</t>
+    <t>Maestría profesional</t>
+  </si>
+  <si>
+    <t>https://utpl.instructure.com/courses/56814</t>
+  </si>
+  <si>
+    <t>EDUC_7094_NLG_META</t>
   </si>
 </sst>
 </file>
@@ -584,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203FE6DB-C04A-E24B-B012-CF294DC0B84C}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29:R30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,7 +678,7 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -693,49 +690,49 @@
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="I2" s="2">
-        <v>1104483498</v>
+        <v>1103442891</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="O2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2" s="2">
         <v>2</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="S2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>44</v>
@@ -750,24 +747,21 @@
       <c r="X2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AB2" s="3">
-        <v>45841</v>
+        <v>45855</v>
       </c>
       <c r="AC2" s="3">
-        <v>45841</v>
+        <v>45855</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="mailto:vhgonzalez@utpl.edu.ec" xr:uid="{B2A1C3AF-0E8D-1649-8C1A-3C5136D6647F}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{5C99694D-E6EE-5541-9058-BC50378FB35F}"/>
+    <hyperlink ref="V2" r:id="rId1" xr:uid="{20ADFCC0-C973-2140-BA8B-AC8D109168AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Actualización que permite etiquetas 'color' y ajuste en etiquetas <code>
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/GitHub/GD-Posgrados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/Proyectos/Guía impresa/Posgrados (plantilla amarilla)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAF9D05-312A-4645-9E50-7E0F29FCE398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A10DAF4-8B65-B04D-9949-EEF4452ACB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4880" yWindow="760" windowWidth="25480" windowHeight="18660" xr2:uid="{81AB655D-E2F9-5747-8328-0D5F0F7CE3C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Código Banner</t>
   </si>
@@ -141,43 +141,46 @@
     <t>Formativo</t>
   </si>
   <si>
+    <t>SIST_7014</t>
+  </si>
+  <si>
+    <t>Bases de Datos Geoespaciales</t>
+  </si>
+  <si>
+    <t>Pucha Cofrep Franz Leonardo</t>
+  </si>
+  <si>
+    <t>fapucha@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Ingenierías y Arquitectura</t>
+  </si>
+  <si>
+    <t>Especialización en Gestión de Geoinformación con mención en Proyectos de Ingeniería</t>
+  </si>
+  <si>
+    <t>González Jaramillo Víctor Hugo</t>
+  </si>
+  <si>
+    <t>vhgonzalez@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Total 144: ACD_32 APE_16 AA_96</t>
+  </si>
+  <si>
     <t>Unidad de Formación Disciplinar Avanzada</t>
   </si>
   <si>
-    <t>EDUC_7094</t>
-  </si>
-  <si>
-    <t>Una Nueva Mirada a la Orientación y Asesoramiento Familiar</t>
-  </si>
-  <si>
-    <t>Beltrán Guevara Patricia Maricela</t>
-  </si>
-  <si>
-    <t>pmbeltran@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Ciencias Sociales, Educación y Humanidades</t>
-  </si>
-  <si>
-    <t>Maestría en Educación con Mención en Orientación Familiar</t>
-  </si>
-  <si>
-    <t>Carrera Herrera Xiomara Paola</t>
-  </si>
-  <si>
-    <t>xpcarrera@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Total 144: ACD_32 APE_16 AA_96</t>
-  </si>
-  <si>
-    <t>Maestría profesional</t>
-  </si>
-  <si>
-    <t>https://utpl.instructure.com/courses/56814</t>
-  </si>
-  <si>
-    <t>EDUC_7094_NLG_META</t>
+    <t>Especialización</t>
+  </si>
+  <si>
+    <t>https://utpl.instructure.com/courses/72916</t>
+  </si>
+  <si>
+    <t>SIST_7014_META</t>
+  </si>
+  <si>
+    <t>180625 Código banner incorrecto</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203FE6DB-C04A-E24B-B012-CF294DC0B84C}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:AC2"/>
     </sheetView>
   </sheetViews>
@@ -678,7 +681,7 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -690,49 +693,49 @@
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="I2" s="2">
-        <v>1103442891</v>
+        <v>1104483498</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="O2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P2" s="2">
         <v>2</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="S2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>44</v>
@@ -747,21 +750,24 @@
       <c r="X2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="2"/>
+      <c r="Y2" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB2" s="3">
-        <v>45855</v>
+        <v>45841</v>
       </c>
       <c r="AC2" s="3">
-        <v>45855</v>
+        <v>45841</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" xr:uid="{20ADFCC0-C973-2140-BA8B-AC8D109168AE}"/>
+    <hyperlink ref="N2" r:id="rId1" display="mailto:vhgonzalez@utpl.edu.ec" xr:uid="{677B0AB6-3FC5-7842-97DF-9F1DE53B15FB}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{B0832AD5-42E4-4D46-BFCB-C962FA6E0337}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Actualización para permitir diferenciar títulos con padding-left: 60px y no considerarlos en el índice
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/Proyectos/Guía impresa/Posgrados (plantilla amarilla)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A10DAF4-8B65-B04D-9949-EEF4452ACB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75771826-011E-DB40-8A15-7C90DFDBFF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4880" yWindow="760" windowWidth="25480" windowHeight="18660" xr2:uid="{81AB655D-E2F9-5747-8328-0D5F0F7CE3C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Código Banner</t>
   </si>
@@ -135,52 +135,49 @@
     <t>Loja</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Formativo</t>
   </si>
   <si>
-    <t>SIST_7014</t>
-  </si>
-  <si>
-    <t>Bases de Datos Geoespaciales</t>
-  </si>
-  <si>
-    <t>Pucha Cofrep Franz Leonardo</t>
-  </si>
-  <si>
-    <t>fapucha@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Ingenierías y Arquitectura</t>
-  </si>
-  <si>
-    <t>Especialización en Gestión de Geoinformación con mención en Proyectos de Ingeniería</t>
-  </si>
-  <si>
-    <t>González Jaramillo Víctor Hugo</t>
-  </si>
-  <si>
-    <t>vhgonzalez@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Total 144: ACD_32 APE_16 AA_96</t>
-  </si>
-  <si>
     <t>Unidad de Formación Disciplinar Avanzada</t>
   </si>
   <si>
-    <t>Especialización</t>
-  </si>
-  <si>
-    <t>https://utpl.instructure.com/courses/72916</t>
-  </si>
-  <si>
-    <t>SIST_7014_META</t>
-  </si>
-  <si>
-    <t>180625 Código banner incorrecto</t>
+    <t>FILO_7014</t>
+  </si>
+  <si>
+    <t>Bioética</t>
+  </si>
+  <si>
+    <t>Vallejo Delgado Merci Lorena</t>
+  </si>
+  <si>
+    <t>mlvallejo11@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Ciencias de la Salud</t>
+  </si>
+  <si>
+    <t>Maestría en Gerencia de Instituciones de Salud</t>
+  </si>
+  <si>
+    <t>Gloria Alexandra Carrión Figueroa</t>
+  </si>
+  <si>
+    <t>gacarrionx@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Total 144: ACD_32 APE_24 AA_88</t>
+  </si>
+  <si>
+    <t>Trayectoria profesional</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>https://utpl.instructure.com/courses/56724</t>
+  </si>
+  <si>
+    <t>FILO_7014_NLG_META</t>
   </si>
 </sst>
 </file>
@@ -584,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203FE6DB-C04A-E24B-B012-CF294DC0B84C}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AC2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,7 +678,7 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -690,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>34</v>
@@ -701,11 +698,11 @@
       <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="2">
-        <v>1104483498</v>
+        <v>1102094883</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>31</v>
@@ -719,7 +716,7 @@
       <c r="M2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="2" t="s">
         <v>41</v>
       </c>
       <c r="O2" s="2">
@@ -732,16 +729,16 @@
         <v>42</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="2">
+        <v>4</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="2">
-        <v>2</v>
-      </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>45</v>
@@ -750,24 +747,22 @@
       <c r="X2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="AB2" s="3">
-        <v>45841</v>
+        <v>45835</v>
       </c>
       <c r="AC2" s="3">
-        <v>45841</v>
+        <v>45835</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="mailto:vhgonzalez@utpl.edu.ec" xr:uid="{677B0AB6-3FC5-7842-97DF-9F1DE53B15FB}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{B0832AD5-42E4-4D46-BFCB-C962FA6E0337}"/>
+    <hyperlink ref="H2" r:id="rId1" display="http://mlvallejo11utpl.edu.ec/" xr:uid="{56206CC7-5E57-DA47-A4CF-04534ADA2280}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{A6859ABA-D5DC-734E-847C-38933535F0CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Actualización de espacios entre focalizadores
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/Proyectos/Guía impresa/Posgrados (plantilla amarilla)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonnsonpardo/Documents/GitHub/GD-Posgrados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75771826-011E-DB40-8A15-7C90DFDBFF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB8ED25-2645-EE43-9B7E-5A3FB281DF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4880" yWindow="760" windowWidth="25480" windowHeight="18660" xr2:uid="{81AB655D-E2F9-5747-8328-0D5F0F7CE3C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Código Banner</t>
   </si>
@@ -141,43 +141,46 @@
     <t>Unidad de Formación Disciplinar Avanzada</t>
   </si>
   <si>
-    <t>FILO_7014</t>
-  </si>
-  <si>
-    <t>Bioética</t>
-  </si>
-  <si>
-    <t>Vallejo Delgado Merci Lorena</t>
-  </si>
-  <si>
-    <t>mlvallejo11@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Ciencias de la Salud</t>
-  </si>
-  <si>
-    <t>Maestría en Gerencia de Instituciones de Salud</t>
-  </si>
-  <si>
-    <t>Gloria Alexandra Carrión Figueroa</t>
-  </si>
-  <si>
-    <t>gacarrionx@utpl.edu.ec</t>
-  </si>
-  <si>
-    <t>Total 144: ACD_32 APE_24 AA_88</t>
-  </si>
-  <si>
-    <t>Trayectoria profesional</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>https://utpl.instructure.com/courses/56724</t>
-  </si>
-  <si>
-    <t>FILO_7014_NLG_META</t>
+    <t>Ciencias Sociales, Educación y Humanidades</t>
+  </si>
+  <si>
+    <t>EDUC_7117</t>
+  </si>
+  <si>
+    <t>Fundamentos de la Educación y Teorías Pedagógicas</t>
+  </si>
+  <si>
+    <t>Pérez Bravo Digna Dionisia</t>
+  </si>
+  <si>
+    <t>ddperez@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>I354288</t>
+  </si>
+  <si>
+    <t>Maestría en Investigación en Educación</t>
+  </si>
+  <si>
+    <t>Yunga Godoy Deisi Cecibel</t>
+  </si>
+  <si>
+    <t>dcyunga@utpl.edu.ec</t>
+  </si>
+  <si>
+    <t>Total 180: ACD_40 APE_24 AA_116</t>
+  </si>
+  <si>
+    <t>Maestría académica</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>https://utpl.instructure.com/courses/56683</t>
+  </si>
+  <si>
+    <t>EDUC_7117_META</t>
   </si>
 </sst>
 </file>
@@ -581,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203FE6DB-C04A-E24B-B012-CF294DC0B84C}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +681,7 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -690,34 +693,34 @@
         <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="2">
-        <v>1102094883</v>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
@@ -726,43 +729,42 @@
         <v>2</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="S2" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB2" s="3">
-        <v>45835</v>
+        <v>45877</v>
       </c>
       <c r="AC2" s="3">
-        <v>45835</v>
+        <v>45877</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="http://mlvallejo11utpl.edu.ec/" xr:uid="{56206CC7-5E57-DA47-A4CF-04534ADA2280}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{A6859ABA-D5DC-734E-847C-38933535F0CD}"/>
+    <hyperlink ref="V2" r:id="rId1" xr:uid="{3942481E-0FBA-3341-9679-C7EB92B01241}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>